<commit_message>
All results, tables, etc updated after changing Indonesian PoS and PUD tests data
</commit_message>
<xml_diff>
--- a/data_exploration/acl/tables/basic_stats_pos_mbert.xlsx
+++ b/data_exploration/acl/tables/basic_stats_pos_mbert.xlsx
@@ -561,7 +561,7 @@
         <v>18434</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>18459</v>
       </c>
       <c r="E2">
         <v>29.22009343341557</v>
@@ -570,7 +570,7 @@
         <v>28.16176630139959</v>
       </c>
       <c r="G2">
-        <v>29.874</v>
+        <v>28.95454791700525</v>
       </c>
       <c r="H2">
         <v>2951</v>
@@ -585,10 +585,10 @@
         <v>0.6179522050183575</v>
       </c>
       <c r="L2">
-        <v>3194</v>
+        <v>2922</v>
       </c>
       <c r="M2">
-        <v>10.6915712659838</v>
+        <v>0.5467077788920655</v>
       </c>
       <c r="N2">
         <v>3</v>
@@ -603,10 +603,10 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>0.4217714400482024</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -620,7 +620,7 @@
         <v>1654</v>
       </c>
       <c r="D3">
-        <v>1000</v>
+        <v>1721</v>
       </c>
       <c r="E3">
         <v>40.33526738902481</v>
@@ -629,7 +629,7 @@
         <v>41.35610640870617</v>
       </c>
       <c r="G3">
-        <v>29.489</v>
+        <v>39.78675188843695</v>
       </c>
       <c r="H3">
         <v>3313</v>
@@ -644,10 +644,10 @@
         <v>4.324371738081663</v>
       </c>
       <c r="L3">
-        <v>3070</v>
+        <v>3036</v>
       </c>
       <c r="M3">
-        <v>10.41066160263149</v>
+        <v>4.433864442919107</v>
       </c>
       <c r="N3">
         <v>29</v>
@@ -662,10 +662,10 @@
         <v>0.004385772553835358</v>
       </c>
       <c r="R3">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="S3">
-        <v>0.01356437993828207</v>
+        <v>0.01898558555927154</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -856,7 +856,7 @@
         <v>500</v>
       </c>
       <c r="D7">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E7">
         <v>37.07705779334501</v>
@@ -865,7 +865,7 @@
         <v>38.18</v>
       </c>
       <c r="G7">
-        <v>33.63</v>
+        <v>36.376</v>
       </c>
       <c r="H7">
         <v>2260</v>
@@ -880,10 +880,10 @@
         <v>6.296490309062336</v>
       </c>
       <c r="L7">
-        <v>1366</v>
+        <v>1189</v>
       </c>
       <c r="M7">
-        <v>4.061849539101992</v>
+        <v>6.537277325709259</v>
       </c>
       <c r="N7">
         <v>126</v>
@@ -898,10 +898,10 @@
         <v>0.07333682556312204</v>
       </c>
       <c r="R7">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="S7">
-        <v>0.5798394290811775</v>
+        <v>0.04948317572025512</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -1014,58 +1014,58 @@
         <v>28</v>
       </c>
       <c r="B11">
-        <v>656</v>
+        <v>4477</v>
       </c>
       <c r="C11">
-        <v>374</v>
+        <v>559</v>
       </c>
       <c r="D11">
-        <v>1000</v>
+        <v>557</v>
       </c>
       <c r="E11">
-        <v>44.11432926829269</v>
+        <v>30.61000670091579</v>
       </c>
       <c r="F11">
-        <v>41.75401069518717</v>
+        <v>31.83184257602862</v>
       </c>
       <c r="G11">
-        <v>28.221</v>
+        <v>29.7181328545781</v>
       </c>
       <c r="H11">
-        <v>1380</v>
+        <v>4257</v>
       </c>
       <c r="I11">
-        <v>4.768651301012475</v>
+        <v>3.106369626608096</v>
       </c>
       <c r="J11">
-        <v>1297</v>
+        <v>2366</v>
       </c>
       <c r="K11">
-        <v>8.305584016393443</v>
+        <v>13.29661683713611</v>
       </c>
       <c r="L11">
-        <v>2144</v>
+        <v>2257</v>
       </c>
       <c r="M11">
-        <v>7.597179405407322</v>
+        <v>13.63499063613846</v>
       </c>
       <c r="N11">
-        <v>3</v>
+        <v>168</v>
       </c>
       <c r="O11">
-        <v>0.0103666332630706</v>
+        <v>0.122591049393977</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>0.1966955153422502</v>
       </c>
       <c r="R11">
-        <v>118</v>
+        <v>21</v>
       </c>
       <c r="S11">
-        <v>0.418128344140888</v>
+        <v>0.1268652208058962</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1079,7 +1079,7 @@
         <v>1364</v>
       </c>
       <c r="D12">
-        <v>1000</v>
+        <v>1555</v>
       </c>
       <c r="E12">
         <v>30.00654825243513</v>
@@ -1088,7 +1088,7 @@
         <v>29.88636363636364</v>
       </c>
       <c r="G12">
-        <v>33.789</v>
+        <v>29.97041800643087</v>
       </c>
       <c r="H12">
         <v>3119</v>
@@ -1103,10 +1103,10 @@
         <v>3.868514657181406</v>
       </c>
       <c r="L12">
-        <v>2033</v>
+        <v>1600</v>
       </c>
       <c r="M12">
-        <v>6.016751013643494</v>
+        <v>3.433181701141533</v>
       </c>
       <c r="N12">
         <v>840</v>
@@ -1121,10 +1121,10 @@
         <v>0.1962467803262603</v>
       </c>
       <c r="R12">
-        <v>195</v>
+        <v>93</v>
       </c>
       <c r="S12">
-        <v>0.5771108940779544</v>
+        <v>0.1995536863788516</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1256,7 +1256,7 @@
         <v>501</v>
       </c>
       <c r="D15">
-        <v>1000</v>
+        <v>543</v>
       </c>
       <c r="E15">
         <v>34.95318058915611</v>
@@ -1265,7 +1265,7 @@
         <v>35.54890219560878</v>
       </c>
       <c r="G15">
-        <v>41.66</v>
+        <v>35.51565377532228</v>
       </c>
       <c r="H15">
         <v>1668</v>
@@ -1280,10 +1280,10 @@
         <v>5.732734418865806</v>
       </c>
       <c r="L15">
-        <v>1027</v>
+        <v>929</v>
       </c>
       <c r="M15">
-        <v>2.465194431108977</v>
+        <v>4.817215452424164</v>
       </c>
       <c r="N15">
         <v>548</v>
@@ -1298,10 +1298,10 @@
         <v>0.2358225715889949</v>
       </c>
       <c r="R15">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="S15">
-        <v>0.009601536245799328</v>
+        <v>0.3266787658802178</v>
       </c>
     </row>
     <row r="16" spans="1:19">

</xml_diff>

<commit_message>
Added shortest and longest example to basic stats
</commit_message>
<xml_diff>
--- a/data_exploration/acl/tables/basic_stats_pos_mbert.xlsx
+++ b/data_exploration/acl/tables/basic_stats_pos_mbert.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>language</t>
   </si>
@@ -35,6 +35,24 @@
   </si>
   <si>
     <t>test_avg_tokens</t>
+  </si>
+  <si>
+    <t>train_longest</t>
+  </si>
+  <si>
+    <t>dev_longest</t>
+  </si>
+  <si>
+    <t>test_longest</t>
+  </si>
+  <si>
+    <t>train_shortest</t>
+  </si>
+  <si>
+    <t>dev_shortest</t>
+  </si>
+  <si>
+    <t>test_shortest</t>
   </si>
   <si>
     <t>train_hapaxes</t>
@@ -485,13 +503,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,10 +567,28 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>38102</v>
@@ -573,45 +609,63 @@
         <v>28.95454791700525</v>
       </c>
       <c r="H2">
+        <v>151</v>
+      </c>
+      <c r="I2">
+        <v>153</v>
+      </c>
+      <c r="J2">
+        <v>128</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
         <v>2951</v>
       </c>
-      <c r="I2">
+      <c r="O2">
         <v>0.2650573407679926</v>
       </c>
-      <c r="J2">
+      <c r="P2">
         <v>3208</v>
       </c>
-      <c r="K2">
+      <c r="Q2">
         <v>0.6179522050183575</v>
       </c>
-      <c r="L2">
+      <c r="R2">
         <v>2922</v>
       </c>
-      <c r="M2">
+      <c r="S2">
         <v>0.5467077788920655</v>
       </c>
-      <c r="N2">
-        <v>3</v>
-      </c>
-      <c r="O2">
+      <c r="T2">
+        <v>3</v>
+      </c>
+      <c r="U2">
         <v>0.0002694584962060244</v>
       </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>14305</v>
@@ -632,45 +686,63 @@
         <v>39.78675188843695</v>
       </c>
       <c r="H3">
+        <v>187</v>
+      </c>
+      <c r="I3">
+        <v>165</v>
+      </c>
+      <c r="J3">
+        <v>194</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
         <v>3313</v>
       </c>
-      <c r="I3">
+      <c r="O3">
         <v>0.5741807568856629</v>
       </c>
-      <c r="J3">
+      <c r="P3">
         <v>2958</v>
       </c>
-      <c r="K3">
+      <c r="Q3">
         <v>4.324371738081663</v>
       </c>
-      <c r="L3">
+      <c r="R3">
         <v>3036</v>
       </c>
-      <c r="M3">
+      <c r="S3">
         <v>4.433864442919107</v>
       </c>
-      <c r="N3">
+      <c r="T3">
         <v>29</v>
       </c>
-      <c r="O3">
+      <c r="U3">
         <v>0.005026031376300702</v>
       </c>
-      <c r="P3">
-        <v>3</v>
-      </c>
-      <c r="Q3">
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3">
         <v>0.004385772553835358</v>
       </c>
-      <c r="R3">
+      <c r="X3">
         <v>13</v>
       </c>
-      <c r="S3">
+      <c r="Y3">
         <v>0.01898558555927154</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>8483</v>
@@ -691,45 +763,63 @@
         <v>24.9679547596607</v>
       </c>
       <c r="H4">
+        <v>97</v>
+      </c>
+      <c r="I4">
+        <v>93</v>
+      </c>
+      <c r="J4">
+        <v>92</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
         <v>1805</v>
       </c>
-      <c r="I4">
+      <c r="O4">
         <v>1.160921018780551</v>
       </c>
-      <c r="J4">
+      <c r="P4">
         <v>1863</v>
       </c>
-      <c r="K4">
+      <c r="Q4">
         <v>7.490952955367913</v>
       </c>
-      <c r="L4">
+      <c r="R4">
         <v>1641</v>
       </c>
-      <c r="M4">
+      <c r="S4">
         <v>6.194556641878374</v>
       </c>
-      <c r="N4">
+      <c r="T4">
         <v>2106</v>
       </c>
-      <c r="O4">
+      <c r="U4">
         <v>1.354515050167224</v>
       </c>
-      <c r="P4">
+      <c r="V4">
         <v>59</v>
       </c>
-      <c r="Q4">
+      <c r="W4">
         <v>0.2372336147969441</v>
       </c>
-      <c r="R4">
+      <c r="X4">
         <v>37</v>
       </c>
-      <c r="S4">
+      <c r="Y4">
         <v>0.1396700766297988</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>15696</v>
@@ -750,45 +840,63 @@
         <v>23.43991748323878</v>
       </c>
       <c r="H5">
+        <v>159</v>
+      </c>
+      <c r="I5">
+        <v>124</v>
+      </c>
+      <c r="J5">
+        <v>106</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
         <v>2863</v>
       </c>
-      <c r="I5">
+      <c r="O5">
         <v>0.787053073163222</v>
       </c>
-      <c r="J5">
+      <c r="P5">
         <v>1882</v>
       </c>
-      <c r="K5">
+      <c r="Q5">
         <v>3.435936758315989</v>
       </c>
-      <c r="L5">
+      <c r="R5">
         <v>1681</v>
       </c>
-      <c r="M5">
+      <c r="S5">
         <v>3.698569856985698</v>
       </c>
-      <c r="N5">
+      <c r="T5">
         <v>88</v>
       </c>
-      <c r="O5">
+      <c r="U5">
         <v>0.02419164178776233</v>
       </c>
-      <c r="P5">
+      <c r="V5">
         <v>2</v>
       </c>
-      <c r="Q5">
+      <c r="W5">
         <v>0.003651367437105196</v>
       </c>
-      <c r="R5">
+      <c r="X5">
         <v>1</v>
       </c>
-      <c r="S5">
+      <c r="Y5">
         <v>0.0022002200220022</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>1662</v>
@@ -809,45 +917,63 @@
         <v>57.44736842105263</v>
       </c>
       <c r="H6">
+        <v>258</v>
+      </c>
+      <c r="I6">
+        <v>195</v>
+      </c>
+      <c r="J6">
+        <v>268</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
         <v>356</v>
       </c>
-      <c r="I6">
+      <c r="O6">
         <v>0.3431325301204819</v>
       </c>
-      <c r="J6">
+      <c r="P6">
         <v>286</v>
       </c>
-      <c r="K6">
+      <c r="Q6">
         <v>1.137267377127406</v>
       </c>
-      <c r="L6">
+      <c r="R6">
         <v>325</v>
       </c>
-      <c r="M6">
+      <c r="S6">
         <v>1.240647427088105</v>
       </c>
-      <c r="N6">
-        <v>3</v>
-      </c>
-      <c r="O6">
+      <c r="T6">
+        <v>3</v>
+      </c>
+      <c r="U6">
         <v>0.002891566265060241</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
         <v>2</v>
       </c>
-      <c r="S6">
+      <c r="Y6">
         <v>0.007634753397465261</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>3997</v>
@@ -868,45 +994,63 @@
         <v>36.376</v>
       </c>
       <c r="H7">
+        <v>166</v>
+      </c>
+      <c r="I7">
+        <v>132</v>
+      </c>
+      <c r="J7">
+        <v>153</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>11</v>
+      </c>
+      <c r="M7">
+        <v>9</v>
+      </c>
+      <c r="N7">
         <v>2260</v>
       </c>
-      <c r="I7">
+      <c r="O7">
         <v>1.524997132195658</v>
       </c>
-      <c r="J7">
+      <c r="P7">
         <v>1202</v>
       </c>
-      <c r="K7">
+      <c r="Q7">
         <v>6.296490309062336</v>
       </c>
-      <c r="L7">
+      <c r="R7">
         <v>1189</v>
       </c>
-      <c r="M7">
+      <c r="S7">
         <v>6.537277325709259</v>
       </c>
-      <c r="N7">
+      <c r="T7">
         <v>126</v>
       </c>
-      <c r="O7">
+      <c r="U7">
         <v>0.08502196400736857</v>
       </c>
-      <c r="P7">
+      <c r="V7">
         <v>14</v>
       </c>
-      <c r="Q7">
+      <c r="W7">
         <v>0.07333682556312204</v>
       </c>
-      <c r="R7">
+      <c r="X7">
         <v>9</v>
       </c>
-      <c r="S7">
+      <c r="Y7">
         <v>0.04948317572025512</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>1400</v>
@@ -927,45 +1071,63 @@
         <v>20.7825</v>
       </c>
       <c r="H8">
+        <v>58</v>
+      </c>
+      <c r="I8">
+        <v>46</v>
+      </c>
+      <c r="J8">
+        <v>42</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
         <v>344</v>
       </c>
-      <c r="I8">
+      <c r="O8">
         <v>1.190393798878815</v>
       </c>
-      <c r="J8">
+      <c r="P8">
         <v>372</v>
       </c>
-      <c r="K8">
+      <c r="Q8">
         <v>2.328201276755539</v>
       </c>
-      <c r="L8">
+      <c r="R8">
         <v>390</v>
       </c>
-      <c r="M8">
+      <c r="S8">
         <v>2.345723565499819</v>
       </c>
-      <c r="N8">
+      <c r="T8">
         <v>15</v>
       </c>
-      <c r="O8">
+      <c r="U8">
         <v>0.05190670634645995</v>
       </c>
-      <c r="P8">
+      <c r="V8">
         <v>1</v>
       </c>
-      <c r="Q8">
+      <c r="W8">
         <v>0.006258605582676179</v>
       </c>
-      <c r="R8">
+      <c r="X8">
         <v>1</v>
       </c>
-      <c r="S8">
+      <c r="Y8">
         <v>0.006014675808973896</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D9">
         <v>1000</v>
@@ -973,22 +1135,28 @@
       <c r="G9">
         <v>69.42400000000001</v>
       </c>
-      <c r="L9">
+      <c r="J9">
+        <v>180</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="R9">
         <v>184</v>
       </c>
-      <c r="M9">
+      <c r="S9">
         <v>0.2650380271952063</v>
       </c>
-      <c r="R9">
+      <c r="X9">
         <v>127</v>
       </c>
-      <c r="S9">
+      <c r="Y9">
         <v>0.1829338557271261</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>1004</v>
@@ -996,22 +1164,28 @@
       <c r="G10">
         <v>17.86653386454183</v>
       </c>
-      <c r="L10">
+      <c r="J10">
+        <v>102</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="R10">
         <v>517</v>
       </c>
-      <c r="M10">
+      <c r="S10">
         <v>2.882149626491247</v>
       </c>
-      <c r="R10">
+      <c r="X10">
         <v>1415</v>
       </c>
-      <c r="S10">
+      <c r="Y10">
         <v>7.888281859739102</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B11">
         <v>4477</v>
@@ -1032,45 +1206,63 @@
         <v>29.7181328545781</v>
       </c>
       <c r="H11">
+        <v>256</v>
+      </c>
+      <c r="I11">
+        <v>226</v>
+      </c>
+      <c r="J11">
+        <v>238</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
+      <c r="N11">
         <v>4257</v>
       </c>
-      <c r="I11">
+      <c r="O11">
         <v>3.106369626608096</v>
       </c>
-      <c r="J11">
+      <c r="P11">
         <v>2366</v>
       </c>
-      <c r="K11">
+      <c r="Q11">
         <v>13.29661683713611</v>
       </c>
-      <c r="L11">
+      <c r="R11">
         <v>2257</v>
       </c>
-      <c r="M11">
+      <c r="S11">
         <v>13.63499063613846</v>
       </c>
-      <c r="N11">
+      <c r="T11">
         <v>168</v>
       </c>
-      <c r="O11">
+      <c r="U11">
         <v>0.122591049393977</v>
       </c>
-      <c r="P11">
+      <c r="V11">
         <v>35</v>
       </c>
-      <c r="Q11">
+      <c r="W11">
         <v>0.1966955153422502</v>
       </c>
-      <c r="R11">
+      <c r="X11">
         <v>21</v>
       </c>
-      <c r="S11">
+      <c r="Y11">
         <v>0.1268652208058962</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <v>12217</v>
@@ -1091,45 +1283,63 @@
         <v>29.97041800643087</v>
       </c>
       <c r="H12">
+        <v>552</v>
+      </c>
+      <c r="I12">
+        <v>463</v>
+      </c>
+      <c r="J12">
+        <v>170</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
         <v>3119</v>
       </c>
-      <c r="I12">
+      <c r="O12">
         <v>0.8508142611636978</v>
       </c>
-      <c r="J12">
+      <c r="P12">
         <v>1577</v>
       </c>
-      <c r="K12">
+      <c r="Q12">
         <v>3.868514657181406</v>
       </c>
-      <c r="L12">
+      <c r="R12">
         <v>1600</v>
       </c>
-      <c r="M12">
+      <c r="S12">
         <v>3.433181701141533</v>
       </c>
-      <c r="N12">
+      <c r="T12">
         <v>840</v>
       </c>
-      <c r="O12">
+      <c r="U12">
         <v>0.2291388199350773</v>
       </c>
-      <c r="P12">
+      <c r="V12">
         <v>80</v>
       </c>
-      <c r="Q12">
+      <c r="W12">
         <v>0.1962467803262603</v>
       </c>
-      <c r="R12">
+      <c r="X12">
         <v>93</v>
       </c>
-      <c r="S12">
+      <c r="Y12">
         <v>0.1995536863788516</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B13">
         <v>5396</v>
@@ -1150,45 +1360,63 @@
         <v>26.11506392440245</v>
       </c>
       <c r="H13">
+        <v>118</v>
+      </c>
+      <c r="I13">
+        <v>89</v>
+      </c>
+      <c r="J13">
+        <v>81</v>
+      </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
         <v>2169</v>
       </c>
-      <c r="I13">
+      <c r="O13">
         <v>1.547130782124897</v>
       </c>
-      <c r="J13">
+      <c r="P13">
         <v>1750</v>
       </c>
-      <c r="K13">
+      <c r="Q13">
         <v>3.786157807057398</v>
       </c>
-      <c r="L13">
+      <c r="R13">
         <v>1767</v>
       </c>
-      <c r="M13">
+      <c r="S13">
         <v>3.761094910708584</v>
       </c>
-      <c r="N13">
+      <c r="T13">
         <v>14</v>
       </c>
-      <c r="O13">
+      <c r="U13">
         <v>0.009986090802097079</v>
       </c>
-      <c r="P13">
-        <v>3</v>
-      </c>
-      <c r="Q13">
+      <c r="V13">
+        <v>3</v>
+      </c>
+      <c r="W13">
         <v>0.006490556240669826</v>
       </c>
-      <c r="R13">
-        <v>3</v>
-      </c>
-      <c r="S13">
+      <c r="X13">
+        <v>3</v>
+      </c>
+      <c r="Y13">
         <v>0.00638556012004853</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>23010</v>
@@ -1209,45 +1437,63 @@
         <v>28.63839090511587</v>
       </c>
       <c r="H14">
+        <v>82</v>
+      </c>
+      <c r="I14">
+        <v>78</v>
+      </c>
+      <c r="J14">
+        <v>83</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
         <v>1432</v>
       </c>
-      <c r="I14">
+      <c r="O14">
         <v>0.2127789194337584</v>
       </c>
-      <c r="J14">
+      <c r="P14">
         <v>439</v>
       </c>
-      <c r="K14">
+      <c r="Q14">
         <v>0.7305708104509901</v>
       </c>
-      <c r="L14">
+      <c r="R14">
         <v>578</v>
       </c>
-      <c r="M14">
+      <c r="S14">
         <v>0.8824966410162453</v>
       </c>
-      <c r="N14">
+      <c r="T14">
         <v>1552</v>
       </c>
-      <c r="O14">
+      <c r="U14">
         <v>0.230609555140498</v>
       </c>
-      <c r="P14">
+      <c r="V14">
         <v>77</v>
       </c>
-      <c r="Q14">
+      <c r="W14">
         <v>0.1281411216508571</v>
       </c>
-      <c r="R14">
+      <c r="X14">
         <v>136</v>
       </c>
-      <c r="S14">
+      <c r="Y14">
         <v>0.2076462684744106</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <v>7027</v>
@@ -1268,45 +1514,63 @@
         <v>35.51565377532228</v>
       </c>
       <c r="H15">
+        <v>183</v>
+      </c>
+      <c r="I15">
+        <v>138</v>
+      </c>
+      <c r="J15">
+        <v>203</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <v>3</v>
+      </c>
+      <c r="N15">
         <v>1668</v>
       </c>
-      <c r="I15">
+      <c r="O15">
         <v>0.679108852843463</v>
       </c>
-      <c r="J15">
+      <c r="P15">
         <v>1021</v>
       </c>
-      <c r="K15">
+      <c r="Q15">
         <v>5.732734418865806</v>
       </c>
-      <c r="L15">
+      <c r="R15">
         <v>929</v>
       </c>
-      <c r="M15">
+      <c r="S15">
         <v>4.817215452424164</v>
       </c>
-      <c r="N15">
+      <c r="T15">
         <v>548</v>
       </c>
-      <c r="O15">
+      <c r="U15">
         <v>0.2231125008142792</v>
       </c>
-      <c r="P15">
+      <c r="V15">
         <v>42</v>
       </c>
-      <c r="Q15">
+      <c r="W15">
         <v>0.2358225715889949</v>
       </c>
-      <c r="R15">
+      <c r="X15">
         <v>63</v>
       </c>
-      <c r="S15">
+      <c r="Y15">
         <v>0.3266787658802178</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>3664</v>
@@ -1327,45 +1591,63 @@
         <v>21.5381485249237</v>
       </c>
       <c r="H16">
+        <v>136</v>
+      </c>
+      <c r="I16">
+        <v>131</v>
+      </c>
+      <c r="J16">
+        <v>94</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
         <v>1138</v>
       </c>
-      <c r="I16">
+      <c r="O16">
         <v>1.424333829805875</v>
       </c>
-      <c r="J16">
+      <c r="P16">
         <v>1042</v>
       </c>
-      <c r="K16">
+      <c r="Q16">
         <v>4.920432544741937</v>
       </c>
-      <c r="L16">
+      <c r="R16">
         <v>985</v>
       </c>
-      <c r="M16">
+      <c r="S16">
         <v>4.652371056111846</v>
       </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B17">
         <v>6075</v>
@@ -1386,45 +1668,63 @@
         <v>89.39705882352941</v>
       </c>
       <c r="H17">
+        <v>932</v>
+      </c>
+      <c r="I17">
+        <v>263</v>
+      </c>
+      <c r="J17">
+        <v>582</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>3</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
         <v>400</v>
       </c>
-      <c r="I17">
+      <c r="O17">
         <v>0.08328492397127503</v>
       </c>
-      <c r="J17">
+      <c r="P17">
         <v>395</v>
       </c>
-      <c r="K17">
+      <c r="Q17">
         <v>0.6219688858096617</v>
       </c>
-      <c r="L17">
+      <c r="R17">
         <v>458</v>
       </c>
-      <c r="M17">
+      <c r="S17">
         <v>0.7534133903602567</v>
       </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
         <v>1</v>
       </c>
-      <c r="S17">
+      <c r="Y17">
         <v>0.001645007402533312</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>5241</v>
@@ -1445,45 +1745,63 @@
         <v>58.54175152749491</v>
       </c>
       <c r="H18">
+        <v>283</v>
+      </c>
+      <c r="I18">
+        <v>229</v>
+      </c>
+      <c r="J18">
+        <v>222</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>4</v>
+      </c>
+      <c r="N18">
         <v>188</v>
       </c>
-      <c r="I18">
+      <c r="O18">
         <v>0.05866054267242455</v>
       </c>
-      <c r="J18">
+      <c r="P18">
         <v>439</v>
       </c>
-      <c r="K18">
+      <c r="Q18">
         <v>1.672317245057331</v>
       </c>
-      <c r="L18">
+      <c r="R18">
         <v>443</v>
       </c>
-      <c r="M18">
+      <c r="S18">
         <v>1.541191205121069</v>
       </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B19">
         <v>997</v>
@@ -1504,45 +1822,63 @@
         <v>31.41258741258741</v>
       </c>
       <c r="H19">
+        <v>185</v>
+      </c>
+      <c r="I19">
+        <v>126</v>
+      </c>
+      <c r="J19">
+        <v>133</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="L19">
+        <v>5</v>
+      </c>
+      <c r="M19">
+        <v>4</v>
+      </c>
+      <c r="N19">
         <v>448</v>
       </c>
-      <c r="I19">
+      <c r="O19">
         <v>1.424709810780728</v>
       </c>
-      <c r="J19">
+      <c r="P19">
         <v>283</v>
       </c>
-      <c r="K19">
+      <c r="Q19">
         <v>6.265220278946202</v>
       </c>
-      <c r="L19">
+      <c r="R19">
         <v>291</v>
       </c>
-      <c r="M19">
+      <c r="S19">
         <v>6.478183437221728</v>
       </c>
-      <c r="N19">
+      <c r="T19">
         <v>125</v>
       </c>
-      <c r="O19">
+      <c r="U19">
         <v>0.3975194784544443</v>
       </c>
-      <c r="P19">
+      <c r="V19">
         <v>12</v>
       </c>
-      <c r="Q19">
+      <c r="W19">
         <v>0.2656630506973655</v>
       </c>
-      <c r="R19">
+      <c r="X19">
         <v>8</v>
       </c>
-      <c r="S19">
+      <c r="Y19">
         <v>0.1780943900267141</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B20">
         <v>1123</v>
@@ -1563,39 +1899,57 @@
         <v>47.5984555984556</v>
       </c>
       <c r="H20">
+        <v>213</v>
+      </c>
+      <c r="I20">
+        <v>152</v>
+      </c>
+      <c r="J20">
+        <v>157</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+      <c r="N20">
         <v>1215</v>
       </c>
-      <c r="I20">
+      <c r="O20">
         <v>2.417092724849305</v>
       </c>
-      <c r="J20">
+      <c r="P20">
         <v>874</v>
       </c>
-      <c r="K20">
+      <c r="Q20">
         <v>3.893616073417383</v>
       </c>
-      <c r="L20">
+      <c r="R20">
         <v>856</v>
       </c>
-      <c r="M20">
+      <c r="S20">
         <v>3.471771576898118</v>
       </c>
-      <c r="N20">
+      <c r="T20">
         <v>470</v>
       </c>
-      <c r="O20">
+      <c r="U20">
         <v>0.9350070622873854</v>
       </c>
-      <c r="P20">
+      <c r="V20">
         <v>191</v>
       </c>
-      <c r="Q20">
+      <c r="W20">
         <v>0.8508932151289705</v>
       </c>
-      <c r="R20">
+      <c r="X20">
         <v>234</v>
       </c>
-      <c r="S20">
+      <c r="Y20">
         <v>0.9490590525632706</v>
       </c>
     </row>

</xml_diff>